<commit_message>
works before moving unit_manager to init.py
</commit_message>
<xml_diff>
--- a/example_5_3/example_5_3_results.xlsx
+++ b/example_5_3/example_5_3_results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
   <si>
     <t>Parameter</t>
   </si>
@@ -96,10 +96,10 @@
     <t>ft</t>
   </si>
   <si>
-    <t>klbf*in</t>
-  </si>
-  <si>
-    <t>klbf/in</t>
+    <t>klbf * foot</t>
+  </si>
+  <si>
+    <t>klbf / foot</t>
   </si>
   <si>
     <t>in^2</t>
@@ -144,7 +144,19 @@
     <t>Reaction Y (klbf)</t>
   </si>
   <si>
-    <t>Moment Z (klbf*in)</t>
+    <t>Moment Z (klbf * foot)</t>
+  </si>
+  <si>
+    <t>0.0 meter</t>
+  </si>
+  <si>
+    <t>359.99999999999994 meter</t>
+  </si>
+  <si>
+    <t>719.9999999999999 meter</t>
+  </si>
+  <si>
+    <t>-0.004894581280788177 radian</t>
   </si>
   <si>
     <t>Member ID</t>
@@ -159,7 +171,7 @@
     <t>Fy (klbf)</t>
   </si>
   <si>
-    <t>Mz (klbf*in)</t>
+    <t>Mz (klbf * foot)</t>
   </si>
   <si>
     <t>System</t>
@@ -177,6 +189,33 @@
     <t>3 (j)</t>
   </si>
   <si>
+    <t>0.0 newton</t>
+  </si>
+  <si>
+    <t>24.25000000000002 newton</t>
+  </si>
+  <si>
+    <t>35.74999999999999 newton</t>
+  </si>
+  <si>
+    <t>37.58333333333336 newton</t>
+  </si>
+  <si>
+    <t>40.416666666666664 newton</t>
+  </si>
+  <si>
+    <t>92.50000000000009 meter * newton</t>
+  </si>
+  <si>
+    <t>-264.9999999999998 meter * newton</t>
+  </si>
+  <si>
+    <t>115.00000000000006 meter * newton</t>
+  </si>
+  <si>
+    <t>-247.49999999999974 meter * newton</t>
+  </si>
+  <si>
     <t>Global</t>
   </si>
   <si>
@@ -214,6 +253,15 @@
   </si>
   <si>
     <t>FRAME</t>
+  </si>
+  <si>
+    <t>29000.00000000001 pascal</t>
+  </si>
+  <si>
+    <t>10.000000000000002 meter ** 2</t>
+  </si>
+  <si>
+    <t>875.0000000000002 meter ** 4</t>
   </si>
   <si>
     <t>None</t>
@@ -299,10 +347,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>97024</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>166507</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>526097</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>187615</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -320,7 +368,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6193024" cy="2643007"/>
+          <a:ext cx="7231697" cy="1711615"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -840,11 +888,11 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -878,11 +926,11 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>359.9999999999999</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -899,8 +947,8 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3">
-        <v>0</v>
+      <c r="I3" t="s">
+        <v>45</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -916,11 +964,11 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>719.9999999999999</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -965,22 +1013,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -988,19 +1036,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1008,19 +1056,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1028,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1040,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1048,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1060,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1068,19 +1116,19 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1088,19 +1136,19 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1108,7 +1156,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1120,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1128,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1140,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1158,37 +1206,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1196,7 +1244,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1204,26 +1252,26 @@
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2">
-        <v>359.9999999999999</v>
+      <c r="E2" t="s">
+        <v>43</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>29000.00000000001</v>
+      <c r="G2" t="s">
+        <v>78</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <v>875.0000000000002</v>
+      <c r="I2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" t="s">
+        <v>80</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1231,7 +1279,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1239,26 +1287,26 @@
       <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3">
-        <v>359.9999999999999</v>
+      <c r="E3" t="s">
+        <v>43</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>29000.00000000001</v>
+      <c r="G3" t="s">
+        <v>78</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>875.0000000000002</v>
+      <c r="I3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" t="s">
+        <v>80</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>